<commit_message>
Added graphs, added data to TCSDB structure
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="723" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="723" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="CorpRiskTable" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7385" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7385" uniqueCount="168">
   <si>
     <t>LocationID</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>Dublin_Ireland</t>
+  </si>
+  <si>
+    <t>Reputation damage</t>
+  </si>
+  <si>
+    <t>Carbon pricing</t>
   </si>
 </sst>
 </file>
@@ -34223,7 +34229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -36189,12 +36195,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H326"/>
   <sheetViews>
-    <sheetView topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -36235,7 +36242,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
@@ -36261,7 +36268,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
@@ -36287,7 +36294,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
@@ -36313,7 +36320,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
@@ -36339,7 +36346,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E6" t="s">
         <v>45</v>
@@ -36365,7 +36372,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -36391,7 +36398,7 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>
@@ -36417,7 +36424,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E9" t="s">
         <v>45</v>
@@ -36443,7 +36450,7 @@
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E10" t="s">
         <v>45</v>
@@ -36703,7 +36710,7 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E20" t="s">
         <v>45</v>
@@ -36729,7 +36736,7 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
@@ -36755,7 +36762,7 @@
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E22" t="s">
         <v>45</v>
@@ -36781,7 +36788,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E23" t="s">
         <v>45</v>
@@ -36807,7 +36814,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E24" t="s">
         <v>45</v>
@@ -36833,7 +36840,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E25" t="s">
         <v>45</v>
@@ -36859,7 +36866,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E26" t="s">
         <v>45</v>
@@ -36885,7 +36892,7 @@
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
@@ -36911,7 +36918,7 @@
         <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E28" t="s">
         <v>45</v>
@@ -37639,7 +37646,7 @@
         <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E56" t="s">
         <v>45</v>
@@ -37665,7 +37672,7 @@
         <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E57" t="s">
         <v>45</v>
@@ -37691,7 +37698,7 @@
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E58" t="s">
         <v>45</v>
@@ -37717,7 +37724,7 @@
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E59" t="s">
         <v>45</v>
@@ -37743,7 +37750,7 @@
         <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E60" t="s">
         <v>45</v>
@@ -37769,7 +37776,7 @@
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E61" t="s">
         <v>45</v>
@@ -37795,7 +37802,7 @@
         <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E62" t="s">
         <v>45</v>
@@ -37821,7 +37828,7 @@
         <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E63" t="s">
         <v>45</v>
@@ -37847,7 +37854,7 @@
         <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E64" t="s">
         <v>45</v>
@@ -38107,7 +38114,7 @@
         <v>23</v>
       </c>
       <c r="D74" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E74" t="s">
         <v>45</v>
@@ -38133,7 +38140,7 @@
         <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E75" t="s">
         <v>45</v>
@@ -38159,7 +38166,7 @@
         <v>23</v>
       </c>
       <c r="D76" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E76" t="s">
         <v>45</v>
@@ -38185,7 +38192,7 @@
         <v>23</v>
       </c>
       <c r="D77" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E77" t="s">
         <v>45</v>
@@ -38211,7 +38218,7 @@
         <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E78" t="s">
         <v>45</v>
@@ -38237,7 +38244,7 @@
         <v>23</v>
       </c>
       <c r="D79" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E79" t="s">
         <v>45</v>
@@ -38263,7 +38270,7 @@
         <v>23</v>
       </c>
       <c r="D80" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E80" t="s">
         <v>45</v>
@@ -38289,7 +38296,7 @@
         <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E81" t="s">
         <v>45</v>
@@ -38315,7 +38322,7 @@
         <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E82" t="s">
         <v>45</v>
@@ -39043,7 +39050,7 @@
         <v>20</v>
       </c>
       <c r="D110" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E110" t="s">
         <v>45</v>
@@ -39069,7 +39076,7 @@
         <v>20</v>
       </c>
       <c r="D111" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E111" t="s">
         <v>45</v>
@@ -39095,7 +39102,7 @@
         <v>20</v>
       </c>
       <c r="D112" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E112" t="s">
         <v>45</v>
@@ -39121,7 +39128,7 @@
         <v>20</v>
       </c>
       <c r="D113" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E113" t="s">
         <v>45</v>
@@ -39147,7 +39154,7 @@
         <v>20</v>
       </c>
       <c r="D114" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E114" t="s">
         <v>45</v>
@@ -39173,7 +39180,7 @@
         <v>20</v>
       </c>
       <c r="D115" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E115" t="s">
         <v>45</v>
@@ -39199,7 +39206,7 @@
         <v>20</v>
       </c>
       <c r="D116" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E116" t="s">
         <v>45</v>
@@ -39225,7 +39232,7 @@
         <v>20</v>
       </c>
       <c r="D117" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E117" t="s">
         <v>45</v>
@@ -39251,7 +39258,7 @@
         <v>20</v>
       </c>
       <c r="D118" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E118" t="s">
         <v>45</v>
@@ -39511,7 +39518,7 @@
         <v>23</v>
       </c>
       <c r="D128" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E128" t="s">
         <v>45</v>
@@ -39537,7 +39544,7 @@
         <v>23</v>
       </c>
       <c r="D129" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E129" t="s">
         <v>45</v>
@@ -39563,7 +39570,7 @@
         <v>23</v>
       </c>
       <c r="D130" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E130" t="s">
         <v>45</v>
@@ -39589,7 +39596,7 @@
         <v>23</v>
       </c>
       <c r="D131" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E131" t="s">
         <v>45</v>
@@ -39615,7 +39622,7 @@
         <v>23</v>
       </c>
       <c r="D132" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E132" t="s">
         <v>45</v>
@@ -39641,7 +39648,7 @@
         <v>23</v>
       </c>
       <c r="D133" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E133" t="s">
         <v>45</v>
@@ -39667,7 +39674,7 @@
         <v>23</v>
       </c>
       <c r="D134" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E134" t="s">
         <v>45</v>
@@ -39693,7 +39700,7 @@
         <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E135" t="s">
         <v>45</v>
@@ -39719,7 +39726,7 @@
         <v>23</v>
       </c>
       <c r="D136" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E136" t="s">
         <v>45</v>
@@ -40447,7 +40454,7 @@
         <v>20</v>
       </c>
       <c r="D164" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E164" t="s">
         <v>45</v>
@@ -40473,7 +40480,7 @@
         <v>20</v>
       </c>
       <c r="D165" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E165" t="s">
         <v>45</v>
@@ -40499,7 +40506,7 @@
         <v>20</v>
       </c>
       <c r="D166" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E166" t="s">
         <v>45</v>
@@ -40525,7 +40532,7 @@
         <v>20</v>
       </c>
       <c r="D167" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E167" t="s">
         <v>45</v>
@@ -40551,7 +40558,7 @@
         <v>20</v>
       </c>
       <c r="D168" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E168" t="s">
         <v>45</v>
@@ -40577,7 +40584,7 @@
         <v>20</v>
       </c>
       <c r="D169" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E169" t="s">
         <v>45</v>
@@ -40603,7 +40610,7 @@
         <v>20</v>
       </c>
       <c r="D170" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E170" t="s">
         <v>45</v>
@@ -40629,7 +40636,7 @@
         <v>20</v>
       </c>
       <c r="D171" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E171" t="s">
         <v>45</v>
@@ -40655,7 +40662,7 @@
         <v>20</v>
       </c>
       <c r="D172" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E172" t="s">
         <v>45</v>
@@ -40915,7 +40922,7 @@
         <v>23</v>
       </c>
       <c r="D182" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E182" t="s">
         <v>45</v>
@@ -40941,7 +40948,7 @@
         <v>23</v>
       </c>
       <c r="D183" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E183" t="s">
         <v>45</v>
@@ -40967,7 +40974,7 @@
         <v>23</v>
       </c>
       <c r="D184" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E184" t="s">
         <v>45</v>
@@ -40993,7 +41000,7 @@
         <v>23</v>
       </c>
       <c r="D185" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E185" t="s">
         <v>45</v>
@@ -41019,7 +41026,7 @@
         <v>23</v>
       </c>
       <c r="D186" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E186" t="s">
         <v>45</v>
@@ -41045,7 +41052,7 @@
         <v>23</v>
       </c>
       <c r="D187" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E187" t="s">
         <v>45</v>
@@ -41071,7 +41078,7 @@
         <v>23</v>
       </c>
       <c r="D188" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E188" t="s">
         <v>45</v>
@@ -41097,7 +41104,7 @@
         <v>23</v>
       </c>
       <c r="D189" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E189" t="s">
         <v>45</v>
@@ -41123,7 +41130,7 @@
         <v>23</v>
       </c>
       <c r="D190" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E190" t="s">
         <v>45</v>
@@ -41851,7 +41858,7 @@
         <v>20</v>
       </c>
       <c r="D218" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E218" t="s">
         <v>45</v>
@@ -41877,7 +41884,7 @@
         <v>20</v>
       </c>
       <c r="D219" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E219" t="s">
         <v>45</v>
@@ -41903,7 +41910,7 @@
         <v>20</v>
       </c>
       <c r="D220" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E220" t="s">
         <v>45</v>
@@ -41929,7 +41936,7 @@
         <v>20</v>
       </c>
       <c r="D221" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E221" t="s">
         <v>45</v>
@@ -41955,7 +41962,7 @@
         <v>20</v>
       </c>
       <c r="D222" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E222" t="s">
         <v>45</v>
@@ -41981,7 +41988,7 @@
         <v>20</v>
       </c>
       <c r="D223" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E223" t="s">
         <v>45</v>
@@ -42007,7 +42014,7 @@
         <v>20</v>
       </c>
       <c r="D224" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E224" t="s">
         <v>45</v>
@@ -42033,7 +42040,7 @@
         <v>20</v>
       </c>
       <c r="D225" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E225" t="s">
         <v>45</v>
@@ -42059,7 +42066,7 @@
         <v>20</v>
       </c>
       <c r="D226" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E226" t="s">
         <v>45</v>
@@ -42319,7 +42326,7 @@
         <v>23</v>
       </c>
       <c r="D236" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E236" t="s">
         <v>45</v>
@@ -42345,7 +42352,7 @@
         <v>23</v>
       </c>
       <c r="D237" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E237" t="s">
         <v>45</v>
@@ -42371,7 +42378,7 @@
         <v>23</v>
       </c>
       <c r="D238" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E238" t="s">
         <v>45</v>
@@ -42397,7 +42404,7 @@
         <v>23</v>
       </c>
       <c r="D239" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E239" t="s">
         <v>45</v>
@@ -42423,7 +42430,7 @@
         <v>23</v>
       </c>
       <c r="D240" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E240" t="s">
         <v>45</v>
@@ -42449,7 +42456,7 @@
         <v>23</v>
       </c>
       <c r="D241" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E241" t="s">
         <v>45</v>
@@ -42475,7 +42482,7 @@
         <v>23</v>
       </c>
       <c r="D242" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E242" t="s">
         <v>45</v>
@@ -42501,7 +42508,7 @@
         <v>23</v>
       </c>
       <c r="D243" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E243" t="s">
         <v>45</v>
@@ -42527,7 +42534,7 @@
         <v>23</v>
       </c>
       <c r="D244" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E244" t="s">
         <v>45</v>
@@ -43255,7 +43262,7 @@
         <v>20</v>
       </c>
       <c r="D272" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E272" t="s">
         <v>45</v>
@@ -43281,7 +43288,7 @@
         <v>20</v>
       </c>
       <c r="D273" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E273" t="s">
         <v>45</v>
@@ -43307,7 +43314,7 @@
         <v>20</v>
       </c>
       <c r="D274" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E274" t="s">
         <v>45</v>
@@ -43333,7 +43340,7 @@
         <v>20</v>
       </c>
       <c r="D275" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E275" t="s">
         <v>45</v>
@@ -43359,7 +43366,7 @@
         <v>20</v>
       </c>
       <c r="D276" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E276" t="s">
         <v>45</v>
@@ -43385,7 +43392,7 @@
         <v>20</v>
       </c>
       <c r="D277" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E277" t="s">
         <v>45</v>
@@ -43411,7 +43418,7 @@
         <v>20</v>
       </c>
       <c r="D278" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E278" t="s">
         <v>45</v>
@@ -43437,7 +43444,7 @@
         <v>20</v>
       </c>
       <c r="D279" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E279" t="s">
         <v>45</v>
@@ -43463,7 +43470,7 @@
         <v>20</v>
       </c>
       <c r="D280" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="E280" t="s">
         <v>45</v>
@@ -43723,7 +43730,7 @@
         <v>23</v>
       </c>
       <c r="D290" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E290" t="s">
         <v>45</v>
@@ -43749,7 +43756,7 @@
         <v>23</v>
       </c>
       <c r="D291" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E291" t="s">
         <v>45</v>
@@ -43775,7 +43782,7 @@
         <v>23</v>
       </c>
       <c r="D292" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E292" t="s">
         <v>45</v>
@@ -43801,7 +43808,7 @@
         <v>23</v>
       </c>
       <c r="D293" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E293" t="s">
         <v>45</v>
@@ -43827,7 +43834,7 @@
         <v>23</v>
       </c>
       <c r="D294" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E294" t="s">
         <v>45</v>
@@ -43853,7 +43860,7 @@
         <v>23</v>
       </c>
       <c r="D295" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E295" t="s">
         <v>45</v>
@@ -43879,7 +43886,7 @@
         <v>23</v>
       </c>
       <c r="D296" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E296" t="s">
         <v>45</v>
@@ -43905,7 +43912,7 @@
         <v>23</v>
       </c>
       <c r="D297" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E297" t="s">
         <v>45</v>
@@ -43931,7 +43938,7 @@
         <v>23</v>
       </c>
       <c r="D298" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="E298" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
time series plot (areaByTime)
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="723" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="723" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="CorpRiskTable" sheetId="10" r:id="rId1"/>
@@ -36196,11 +36196,12 @@
   <dimension ref="A1:H326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
added AMP Capital locations
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14352" uniqueCount="1685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14480" uniqueCount="1711">
   <si>
     <t>LocationID</t>
   </si>
@@ -5093,6 +5093,84 @@
   </si>
   <si>
     <t>carbonprice_100</t>
+  </si>
+  <si>
+    <t>AMP Capital</t>
+  </si>
+  <si>
+    <t>ASX</t>
+  </si>
+  <si>
+    <t>AXA</t>
+  </si>
+  <si>
+    <t>AMPC</t>
+  </si>
+  <si>
+    <t>NAB_Headquarters</t>
+  </si>
+  <si>
+    <t>Malvern_Central</t>
+  </si>
+  <si>
+    <t>Exchange_Tower</t>
+  </si>
+  <si>
+    <t>Garden_City</t>
+  </si>
+  <si>
+    <t>The_Palms_NZ</t>
+  </si>
+  <si>
+    <t>Indooroopilly_Shopping_Centre</t>
+  </si>
+  <si>
+    <t>Pacific_Fair</t>
+  </si>
+  <si>
+    <t>Stanley_Plaza</t>
+  </si>
+  <si>
+    <t>Coronation_Drive_Office_Park</t>
+  </si>
+  <si>
+    <t>Macquarie_Centre</t>
+  </si>
+  <si>
+    <t>AMP_Building</t>
+  </si>
+  <si>
+    <t>Indooroopilly_QLD</t>
+  </si>
+  <si>
+    <t>Broadbeach_QLD</t>
+  </si>
+  <si>
+    <t>South_Brisbane_QLD</t>
+  </si>
+  <si>
+    <t>Milton_QLD</t>
+  </si>
+  <si>
+    <t>North_Ryde_NSW</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>Armadale_VIC</t>
+  </si>
+  <si>
+    <t>Perth_WA</t>
+  </si>
+  <si>
+    <t>Booragoon_WA</t>
+  </si>
+  <si>
+    <t>Christchurch_NZ</t>
   </si>
 </sst>
 </file>
@@ -37021,10 +37099,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37121,6 +37199,23 @@
         <v>HP Inc.</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1685</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -37128,10 +37223,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38616,6 +38711,358 @@
         <v>55</v>
       </c>
       <c r="I46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f>Location!A47</f>
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f>Location!B47</f>
+        <v>4</v>
+      </c>
+      <c r="C47" t="str">
+        <f>Location!C47</f>
+        <v>Indooroopilly_Shopping_Centre</v>
+      </c>
+      <c r="D47">
+        <v>100</v>
+      </c>
+      <c r="E47">
+        <v>90</v>
+      </c>
+      <c r="F47">
+        <v>80</v>
+      </c>
+      <c r="G47">
+        <v>0.1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>55</v>
+      </c>
+      <c r="I47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f>Location!A48</f>
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f>Location!B48</f>
+        <v>4</v>
+      </c>
+      <c r="C48" t="str">
+        <f>Location!C48</f>
+        <v>Pacific_Fair</v>
+      </c>
+      <c r="D48">
+        <v>100</v>
+      </c>
+      <c r="E48">
+        <v>90</v>
+      </c>
+      <c r="F48">
+        <v>80</v>
+      </c>
+      <c r="G48">
+        <v>0.1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f>Location!A49</f>
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f>Location!B49</f>
+        <v>4</v>
+      </c>
+      <c r="C49" t="str">
+        <f>Location!C49</f>
+        <v>Stanley_Plaza</v>
+      </c>
+      <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="E49">
+        <v>90</v>
+      </c>
+      <c r="F49">
+        <v>80</v>
+      </c>
+      <c r="G49">
+        <v>0.1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f>Location!A50</f>
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f>Location!B50</f>
+        <v>4</v>
+      </c>
+      <c r="C50" t="str">
+        <f>Location!C50</f>
+        <v>Coronation_Drive_Office_Park</v>
+      </c>
+      <c r="D50">
+        <v>100</v>
+      </c>
+      <c r="E50">
+        <v>90</v>
+      </c>
+      <c r="F50">
+        <v>80</v>
+      </c>
+      <c r="G50">
+        <v>0.1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>55</v>
+      </c>
+      <c r="I50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f>Location!A51</f>
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f>Location!B51</f>
+        <v>4</v>
+      </c>
+      <c r="C51" t="str">
+        <f>Location!C51</f>
+        <v>Macquarie_Centre</v>
+      </c>
+      <c r="D51">
+        <v>100</v>
+      </c>
+      <c r="E51">
+        <v>90</v>
+      </c>
+      <c r="F51">
+        <v>80</v>
+      </c>
+      <c r="G51">
+        <v>0.1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>55</v>
+      </c>
+      <c r="I51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f>Location!A52</f>
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f>Location!B52</f>
+        <v>4</v>
+      </c>
+      <c r="C52" t="str">
+        <f>Location!C52</f>
+        <v>AMP_Building</v>
+      </c>
+      <c r="D52">
+        <v>100</v>
+      </c>
+      <c r="E52">
+        <v>90</v>
+      </c>
+      <c r="F52">
+        <v>80</v>
+      </c>
+      <c r="G52">
+        <v>0.1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f>Location!A53</f>
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f>Location!B53</f>
+        <v>4</v>
+      </c>
+      <c r="C53" t="str">
+        <f>Location!C53</f>
+        <v>NAB_Headquarters</v>
+      </c>
+      <c r="D53">
+        <v>100</v>
+      </c>
+      <c r="E53">
+        <v>90</v>
+      </c>
+      <c r="F53">
+        <v>80</v>
+      </c>
+      <c r="G53">
+        <v>0.1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f>Location!A54</f>
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f>Location!B54</f>
+        <v>4</v>
+      </c>
+      <c r="C54" t="str">
+        <f>Location!C54</f>
+        <v>Malvern_Central</v>
+      </c>
+      <c r="D54">
+        <v>100</v>
+      </c>
+      <c r="E54">
+        <v>90</v>
+      </c>
+      <c r="F54">
+        <v>80</v>
+      </c>
+      <c r="G54">
+        <v>0.1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f>Location!A55</f>
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f>Location!B55</f>
+        <v>4</v>
+      </c>
+      <c r="C55" t="str">
+        <f>Location!C55</f>
+        <v>Exchange_Tower</v>
+      </c>
+      <c r="D55">
+        <v>100</v>
+      </c>
+      <c r="E55">
+        <v>90</v>
+      </c>
+      <c r="F55">
+        <v>80</v>
+      </c>
+      <c r="G55">
+        <v>0.1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f>Location!A56</f>
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f>Location!B56</f>
+        <v>4</v>
+      </c>
+      <c r="C56" t="str">
+        <f>Location!C56</f>
+        <v>Garden_City</v>
+      </c>
+      <c r="D56">
+        <v>100</v>
+      </c>
+      <c r="E56">
+        <v>90</v>
+      </c>
+      <c r="F56">
+        <v>80</v>
+      </c>
+      <c r="G56">
+        <v>0.1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>55</v>
+      </c>
+      <c r="I56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f>Location!A57</f>
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f>Location!B57</f>
+        <v>4</v>
+      </c>
+      <c r="C57" t="str">
+        <f>Location!C57</f>
+        <v>The_Palms_NZ</v>
+      </c>
+      <c r="D57">
+        <v>100</v>
+      </c>
+      <c r="E57">
+        <v>90</v>
+      </c>
+      <c r="F57">
+        <v>80</v>
+      </c>
+      <c r="G57">
+        <v>0.1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>55</v>
+      </c>
+      <c r="I57" t="s">
         <v>55</v>
       </c>
     </row>
@@ -60040,7 +60487,7 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -61703,10 +62150,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView topLeftCell="A52" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -63607,6 +64054,468 @@
         <v>55</v>
       </c>
     </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f>A46+1</f>
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D47">
+        <v>152.97045510000001</v>
+      </c>
+      <c r="E47">
+        <v>-27.499605800000001</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1700</v>
+      </c>
+      <c r="G47" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" t="s">
+        <v>53</v>
+      </c>
+      <c r="I47" t="s">
+        <v>54</v>
+      </c>
+      <c r="J47" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K47" t="s">
+        <v>55</v>
+      </c>
+      <c r="L47" t="s">
+        <v>55</v>
+      </c>
+      <c r="M47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" ref="A48:A57" si="0">A47+1</f>
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D48">
+        <v>153.4258423</v>
+      </c>
+      <c r="E48">
+        <v>-28.036514</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" t="s">
+        <v>53</v>
+      </c>
+      <c r="I48" t="s">
+        <v>54</v>
+      </c>
+      <c r="J48" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K48" t="s">
+        <v>55</v>
+      </c>
+      <c r="L48" t="s">
+        <v>55</v>
+      </c>
+      <c r="M48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D49">
+        <v>153.02070330000001</v>
+      </c>
+      <c r="E49">
+        <v>-27.4786392</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1702</v>
+      </c>
+      <c r="G49" t="s">
+        <v>52</v>
+      </c>
+      <c r="H49" t="s">
+        <v>53</v>
+      </c>
+      <c r="I49" t="s">
+        <v>54</v>
+      </c>
+      <c r="J49" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K49" t="s">
+        <v>55</v>
+      </c>
+      <c r="L49" t="s">
+        <v>55</v>
+      </c>
+      <c r="M49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D50">
+        <v>153.00675190000001</v>
+      </c>
+      <c r="E50">
+        <v>-27.4695483</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1703</v>
+      </c>
+      <c r="G50" t="s">
+        <v>52</v>
+      </c>
+      <c r="H50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I50" t="s">
+        <v>54</v>
+      </c>
+      <c r="J50" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K50" t="s">
+        <v>55</v>
+      </c>
+      <c r="L50" t="s">
+        <v>55</v>
+      </c>
+      <c r="M50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D51">
+        <v>151.11832659999999</v>
+      </c>
+      <c r="E51">
+        <v>-33.776747299999997</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1704</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I51" t="s">
+        <v>54</v>
+      </c>
+      <c r="J51" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K51" t="s">
+        <v>55</v>
+      </c>
+      <c r="L51" t="s">
+        <v>55</v>
+      </c>
+      <c r="M51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D52">
+        <v>151.20993540000001</v>
+      </c>
+      <c r="E52">
+        <v>-33.862573900000001</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1705</v>
+      </c>
+      <c r="G52" t="s">
+        <v>52</v>
+      </c>
+      <c r="H52" t="s">
+        <v>53</v>
+      </c>
+      <c r="I52" t="s">
+        <v>54</v>
+      </c>
+      <c r="J52" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K52" t="s">
+        <v>55</v>
+      </c>
+      <c r="L52" t="s">
+        <v>55</v>
+      </c>
+      <c r="M52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D53">
+        <v>144.94720839999999</v>
+      </c>
+      <c r="E53">
+        <v>-37.817371000000001</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1706</v>
+      </c>
+      <c r="G53" t="s">
+        <v>52</v>
+      </c>
+      <c r="H53" t="s">
+        <v>53</v>
+      </c>
+      <c r="I53" t="s">
+        <v>54</v>
+      </c>
+      <c r="J53" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K53" t="s">
+        <v>55</v>
+      </c>
+      <c r="L53" t="s">
+        <v>55</v>
+      </c>
+      <c r="M53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D54">
+        <v>145.02497679999999</v>
+      </c>
+      <c r="E54">
+        <v>-37.862842499999999</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1707</v>
+      </c>
+      <c r="G54" t="s">
+        <v>52</v>
+      </c>
+      <c r="H54" t="s">
+        <v>53</v>
+      </c>
+      <c r="I54" t="s">
+        <v>54</v>
+      </c>
+      <c r="J54" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K54" t="s">
+        <v>55</v>
+      </c>
+      <c r="L54" t="s">
+        <v>55</v>
+      </c>
+      <c r="M54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D55">
+        <v>115.8564435</v>
+      </c>
+      <c r="E55">
+        <v>-31.956254000000001</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1708</v>
+      </c>
+      <c r="G55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55" t="s">
+        <v>54</v>
+      </c>
+      <c r="J55" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K55" t="s">
+        <v>55</v>
+      </c>
+      <c r="L55" t="s">
+        <v>55</v>
+      </c>
+      <c r="M55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D56">
+        <v>115.83374139999999</v>
+      </c>
+      <c r="E56">
+        <v>-32.0339551</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1709</v>
+      </c>
+      <c r="G56" t="s">
+        <v>52</v>
+      </c>
+      <c r="H56" t="s">
+        <v>53</v>
+      </c>
+      <c r="I56" t="s">
+        <v>54</v>
+      </c>
+      <c r="J56" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K56" t="s">
+        <v>55</v>
+      </c>
+      <c r="L56" t="s">
+        <v>55</v>
+      </c>
+      <c r="M56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D57">
+        <v>172.66268930000001</v>
+      </c>
+      <c r="E57">
+        <v>-43.507471099999997</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1710</v>
+      </c>
+      <c r="G57" t="s">
+        <v>52</v>
+      </c>
+      <c r="H57" t="s">
+        <v>53</v>
+      </c>
+      <c r="I57" t="s">
+        <v>54</v>
+      </c>
+      <c r="J57" t="s">
+        <v>1682</v>
+      </c>
+      <c r="K57" t="s">
+        <v>55</v>
+      </c>
+      <c r="L57" t="s">
+        <v>55</v>
+      </c>
+      <c r="M57" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -63615,10 +64524,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -63682,6 +64591,20 @@
       </c>
       <c r="D4" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed type in coastal-flood DFs; also higher sensitivity for some AMPC locations
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="460" windowWidth="31040" windowHeight="17960" tabRatio="723" activeTab="11"/>
+    <workbookView xWindow="1920" yWindow="1860" windowWidth="31040" windowHeight="17960" tabRatio="723" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CorpRiskTable" sheetId="10" r:id="rId1"/>
@@ -39072,7 +39072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView topLeftCell="D7" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -62149,8 +62149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -62272,7 +62272,7 @@
       <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>59</v>
       </c>
       <c r="J3" t="s">
@@ -64119,8 +64119,8 @@
       <c r="H48" t="s">
         <v>53</v>
       </c>
-      <c r="I48" t="s">
-        <v>54</v>
+      <c r="I48" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="J48" t="s">
         <v>1680</v>
@@ -64287,8 +64287,8 @@
       <c r="H52" t="s">
         <v>53</v>
       </c>
-      <c r="I52" t="s">
-        <v>54</v>
+      <c r="I52" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="J52" t="s">
         <v>1680</v>
@@ -64299,7 +64299,7 @@
       <c r="L52" t="s">
         <v>55</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M52" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -64329,8 +64329,8 @@
       <c r="H53" t="s">
         <v>53</v>
       </c>
-      <c r="I53" t="s">
-        <v>54</v>
+      <c r="I53" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="J53" t="s">
         <v>1680</v>
@@ -64341,7 +64341,7 @@
       <c r="L53" t="s">
         <v>55</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M53" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -64413,8 +64413,8 @@
       <c r="H55" t="s">
         <v>53</v>
       </c>
-      <c r="I55" t="s">
-        <v>54</v>
+      <c r="I55" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="J55" t="s">
         <v>1680</v>
@@ -64425,7 +64425,7 @@
       <c r="L55" t="s">
         <v>55</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M55" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -64455,8 +64455,8 @@
       <c r="H56" t="s">
         <v>53</v>
       </c>
-      <c r="I56" t="s">
-        <v>54</v>
+      <c r="I56" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="J56" t="s">
         <v>1680</v>
@@ -64467,7 +64467,7 @@
       <c r="L56" t="s">
         <v>55</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M56" s="4" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
user data in separate DB linked to SE
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1860" windowWidth="31040" windowHeight="17960" tabRatio="723" activeTab="2"/>
+    <workbookView xWindow="1920" yWindow="1860" windowWidth="31040" windowHeight="17960" tabRatio="723" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="CorpRiskTable" sheetId="10" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="users" sheetId="12" r:id="rId10"/>
     <sheet name="LocationValues" sheetId="13" r:id="rId11"/>
     <sheet name="DamageFunctions" sheetId="14" r:id="rId12"/>
+    <sheet name="BusinessTypes" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14480" uniqueCount="1710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14493" uniqueCount="1723">
   <si>
     <t>LocationID</t>
   </si>
@@ -5168,13 +5169,52 @@
   </si>
   <si>
     <t>0;0.01;0.1;0.2;0.3;0.4;0.5;0.6;0.7;0.8;0.9;1.0</t>
+  </si>
+  <si>
+    <t>BusinessType</t>
+  </si>
+  <si>
+    <t>BusinessTypeID</t>
+  </si>
+  <si>
+    <t>Beverage</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Packaged Foods</t>
+  </si>
+  <si>
+    <t>Paper &amp; Forest</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Metals &amp; Mining</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Oil &amp; Gas</t>
+  </si>
+  <si>
+    <t>Electric Utility</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5207,6 +5247,12 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -5299,7 +5345,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5325,6 +5371,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5727,7 +5774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C904" sqref="C904"/>
     </sheetView>
   </sheetViews>
@@ -37222,7 +37269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -60479,6 +60526,131 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="23" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A12" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G91"/>
@@ -62149,7 +62321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+    <sheetView zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
       <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added risk-factor subsets to corp/port analysis
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="2340" windowWidth="31040" windowHeight="17960" tabRatio="723" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="1420" yWindow="2340" windowWidth="31040" windowHeight="17960" tabRatio="723" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CorpRiskTable" sheetId="10" r:id="rId1"/>
@@ -5738,7 +5738,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5768,6 +5768,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -37719,7 +37722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
@@ -65968,8 +65971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M152"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -67967,11 +67970,11 @@
       <c r="C48" t="s">
         <v>1845</v>
       </c>
-      <c r="D48">
-        <v>-38.6</v>
-      </c>
-      <c r="E48">
-        <v>-7.516667</v>
+      <c r="D48" s="15">
+        <v>-47.368454999999997</v>
+      </c>
+      <c r="E48" s="15">
+        <v>-23.427205000000001</v>
       </c>
       <c r="F48" t="s">
         <v>1845</v>

</xml_diff>

<commit_message>
Additional derived variables; TH Real Estate locations
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="31040" windowHeight="17960" tabRatio="723" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="31460" windowHeight="17980" tabRatio="723" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CorpRiskTable" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15800" uniqueCount="1885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15843" uniqueCount="1894">
   <si>
     <t>LocationID</t>
   </si>
@@ -5696,6 +5696,33 @@
   </si>
   <si>
     <t>Pontevedra_Spain</t>
+  </si>
+  <si>
+    <t>Ginza_1_Chome_Ginza_Japan</t>
+  </si>
+  <si>
+    <t>Xanadu_Centre_Madrid_Spain</t>
+  </si>
+  <si>
+    <t>801_Brickell_Miami_USA</t>
+  </si>
+  <si>
+    <t>TH Real Estate</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>THRE</t>
+  </si>
+  <si>
+    <t>thre</t>
+  </si>
+  <si>
+    <t>Tokyo_Japan</t>
+  </si>
+  <si>
+    <t>Ginza_1_Chome_Tokyo_Japan</t>
   </si>
 </sst>
 </file>
@@ -37655,10 +37682,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37911,6 +37938,23 @@
         <v>1871</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1891</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1888</v>
+      </c>
+      <c r="D15" s="3">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>1888</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -37918,10 +37962,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I164"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView topLeftCell="A155" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <selection activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42803,7 +42847,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="16">
-        <f t="shared" ref="A153:A164" si="0">A152+1</f>
+        <f t="shared" ref="A153:A167" si="0">A152+1</f>
         <v>152</v>
       </c>
       <c r="B153" s="16">
@@ -43158,6 +43202,96 @@
         <v>55</v>
       </c>
       <c r="I164" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="B165" s="14">
+        <v>9</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1887</v>
+      </c>
+      <c r="D165">
+        <v>100</v>
+      </c>
+      <c r="E165">
+        <v>90</v>
+      </c>
+      <c r="F165">
+        <v>80</v>
+      </c>
+      <c r="G165">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="H165" t="s">
+        <v>55</v>
+      </c>
+      <c r="I165" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="B166" s="14">
+        <v>9</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1886</v>
+      </c>
+      <c r="D166">
+        <v>100</v>
+      </c>
+      <c r="E166">
+        <v>90</v>
+      </c>
+      <c r="F166">
+        <v>80</v>
+      </c>
+      <c r="G166">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="H166" t="s">
+        <v>55</v>
+      </c>
+      <c r="I166" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <f t="shared" si="0"/>
+        <v>166</v>
+      </c>
+      <c r="B167" s="14">
+        <v>9</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1885</v>
+      </c>
+      <c r="D167">
+        <v>100</v>
+      </c>
+      <c r="E167">
+        <v>90</v>
+      </c>
+      <c r="F167">
+        <v>80</v>
+      </c>
+      <c r="G167">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="H167" t="s">
+        <v>55</v>
+      </c>
+      <c r="I167" t="s">
         <v>55</v>
       </c>
     </row>
@@ -43170,7 +43304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K617"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -66737,10 +66871,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M164"/>
+  <dimension ref="A1:M170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="H169" sqref="H169"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -72257,7 +72391,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132">
-        <f t="shared" ref="A132:A164" si="2">A131+1</f>
+        <f t="shared" ref="A132:A167" si="2">A131+1</f>
         <v>131</v>
       </c>
       <c r="B132" s="14">
@@ -73640,6 +73774,135 @@
       <c r="M164" s="16" t="s">
         <v>55</v>
       </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+      <c r="B165" s="14">
+        <v>9</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1887</v>
+      </c>
+      <c r="D165">
+        <v>-80.192154599999995</v>
+      </c>
+      <c r="E165">
+        <v>25.7657679</v>
+      </c>
+      <c r="F165" t="s">
+        <v>1763</v>
+      </c>
+      <c r="G165" t="s">
+        <v>52</v>
+      </c>
+      <c r="H165" t="s">
+        <v>53</v>
+      </c>
+      <c r="I165" t="s">
+        <v>54</v>
+      </c>
+      <c r="J165" t="s">
+        <v>1678</v>
+      </c>
+      <c r="K165" t="s">
+        <v>55</v>
+      </c>
+      <c r="L165" t="s">
+        <v>55</v>
+      </c>
+      <c r="M165" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+      <c r="B166" s="14">
+        <v>9</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1886</v>
+      </c>
+      <c r="D166">
+        <v>-3.9283784000000002</v>
+      </c>
+      <c r="E166">
+        <v>40.299783599999998</v>
+      </c>
+      <c r="F166" t="s">
+        <v>1754</v>
+      </c>
+      <c r="G166" t="s">
+        <v>52</v>
+      </c>
+      <c r="H166" t="s">
+        <v>53</v>
+      </c>
+      <c r="I166" t="s">
+        <v>54</v>
+      </c>
+      <c r="J166" t="s">
+        <v>1678</v>
+      </c>
+      <c r="K166" t="s">
+        <v>55</v>
+      </c>
+      <c r="L166" t="s">
+        <v>55</v>
+      </c>
+      <c r="M166" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="B167" s="14">
+        <v>9</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D167">
+        <v>139.7675366</v>
+      </c>
+      <c r="E167">
+        <v>35.673938900000003</v>
+      </c>
+      <c r="F167" t="s">
+        <v>1892</v>
+      </c>
+      <c r="G167" t="s">
+        <v>52</v>
+      </c>
+      <c r="H167" t="s">
+        <v>53</v>
+      </c>
+      <c r="I167" t="s">
+        <v>54</v>
+      </c>
+      <c r="J167" t="s">
+        <v>1678</v>
+      </c>
+      <c r="K167" t="s">
+        <v>55</v>
+      </c>
+      <c r="L167" t="s">
+        <v>55</v>
+      </c>
+      <c r="M167" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" ht="23" x14ac:dyDescent="0.25">
+      <c r="C170" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -73649,10 +73912,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -73786,6 +74049,20 @@
       </c>
       <c r="D9" t="s">
         <v>1872</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1889</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised drought DF assignments
</commit_message>
<xml_diff>
--- a/data/TCSDB/TCSDB_structure.xlsx
+++ b/data/TCSDB/TCSDB_structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="880" yWindow="2940" windowWidth="31460" windowHeight="17980" tabRatio="723" firstSheet="4" activeTab="14"/>
+    <workbookView xWindow="880" yWindow="2940" windowWidth="31460" windowHeight="17980" tabRatio="723" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CorpRiskTable" sheetId="10" r:id="rId1"/>
@@ -47579,7 +47579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K617"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -69442,7 +69442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -69919,7 +69919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -71625,8 +71625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M280"/>
   <sheetViews>
-    <sheetView topLeftCell="A241" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="F246" sqref="F246"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="N231" sqref="N231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71705,7 +71705,7 @@
         <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I2" t="s">
         <v>54</v>
@@ -71747,7 +71747,7 @@
         <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>59</v>
@@ -71789,7 +71789,7 @@
         <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I4" t="s">
         <v>54</v>
@@ -71831,7 +71831,7 @@
         <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I5" t="s">
         <v>54</v>
@@ -71873,7 +71873,7 @@
         <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I6" t="s">
         <v>54</v>
@@ -71915,7 +71915,7 @@
         <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I7" t="s">
         <v>54</v>
@@ -71957,7 +71957,7 @@
         <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I8" t="s">
         <v>54</v>
@@ -71999,7 +71999,7 @@
         <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I9" t="s">
         <v>54</v>
@@ -72965,7 +72965,7 @@
         <v>52</v>
       </c>
       <c r="H32" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I32" t="s">
         <v>54</v>
@@ -73007,7 +73007,7 @@
         <v>52</v>
       </c>
       <c r="H33" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I33" t="s">
         <v>54</v>
@@ -73049,7 +73049,7 @@
         <v>52</v>
       </c>
       <c r="H34" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I34" t="s">
         <v>54</v>
@@ -73091,7 +73091,7 @@
         <v>52</v>
       </c>
       <c r="H35" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I35" t="s">
         <v>54</v>
@@ -73133,7 +73133,7 @@
         <v>52</v>
       </c>
       <c r="H36" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I36" t="s">
         <v>54</v>
@@ -73175,7 +73175,7 @@
         <v>52</v>
       </c>
       <c r="H37" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I37" t="s">
         <v>54</v>
@@ -73217,7 +73217,7 @@
         <v>52</v>
       </c>
       <c r="H38" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I38" t="s">
         <v>54</v>
@@ -73259,7 +73259,7 @@
         <v>52</v>
       </c>
       <c r="H39" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I39" t="s">
         <v>54</v>
@@ -73301,7 +73301,7 @@
         <v>52</v>
       </c>
       <c r="H40" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I40" t="s">
         <v>54</v>
@@ -73343,7 +73343,7 @@
         <v>52</v>
       </c>
       <c r="H41" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I41" t="s">
         <v>54</v>
@@ -73385,7 +73385,7 @@
         <v>52</v>
       </c>
       <c r="H42" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I42" t="s">
         <v>54</v>
@@ -73427,7 +73427,7 @@
         <v>52</v>
       </c>
       <c r="H43" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I43" t="s">
         <v>54</v>
@@ -73469,7 +73469,7 @@
         <v>52</v>
       </c>
       <c r="H44" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I44" t="s">
         <v>54</v>
@@ -73511,7 +73511,7 @@
         <v>52</v>
       </c>
       <c r="H45" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I45" t="s">
         <v>54</v>
@@ -73553,7 +73553,7 @@
         <v>52</v>
       </c>
       <c r="H46" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I46" t="s">
         <v>54</v>
@@ -73595,7 +73595,7 @@
         <v>52</v>
       </c>
       <c r="H47" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I47" t="s">
         <v>54</v>
@@ -73637,7 +73637,7 @@
         <v>52</v>
       </c>
       <c r="H48" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I48" t="s">
         <v>54</v>
@@ -73679,7 +73679,7 @@
         <v>52</v>
       </c>
       <c r="H49" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I49" t="s">
         <v>54</v>
@@ -73721,7 +73721,7 @@
         <v>52</v>
       </c>
       <c r="H50" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I50" t="s">
         <v>54</v>
@@ -73763,7 +73763,7 @@
         <v>52</v>
       </c>
       <c r="H51" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
       <c r="I51" t="s">
         <v>54</v>
@@ -73805,7 +73805,7 @@
         <v>52</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>54</v>
@@ -73847,7 +73847,7 @@
         <v>52</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I53" s="13" t="s">
         <v>59</v>
@@ -73889,7 +73889,7 @@
         <v>52</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I54" s="13" t="s">
         <v>54</v>
@@ -73931,7 +73931,7 @@
         <v>52</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I55" s="13" t="s">
         <v>54</v>
@@ -73973,7 +73973,7 @@
         <v>52</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I56" s="13" t="s">
         <v>54</v>
@@ -74015,7 +74015,7 @@
         <v>52</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I57" s="13" t="s">
         <v>59</v>
@@ -74057,7 +74057,7 @@
         <v>52</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>59</v>
@@ -74099,7 +74099,7 @@
         <v>52</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I59" s="13" t="s">
         <v>54</v>
@@ -74141,7 +74141,7 @@
         <v>52</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>59</v>
@@ -74183,7 +74183,7 @@
         <v>52</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>59</v>
@@ -74225,7 +74225,7 @@
         <v>52</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>54</v>
@@ -74435,7 +74435,7 @@
         <v>52</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>54</v>
@@ -74477,7 +74477,7 @@
         <v>52</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>54</v>
@@ -74519,7 +74519,7 @@
         <v>52</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>54</v>
@@ -74561,7 +74561,7 @@
         <v>52</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>54</v>
@@ -74603,7 +74603,7 @@
         <v>52</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I71" s="13" t="s">
         <v>54</v>
@@ -74645,7 +74645,7 @@
         <v>52</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I72" s="13" t="s">
         <v>54</v>
@@ -74687,7 +74687,7 @@
         <v>52</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I73" s="13" t="s">
         <v>54</v>
@@ -74729,7 +74729,7 @@
         <v>52</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>54</v>
@@ -74771,7 +74771,7 @@
         <v>52</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I75" s="13" t="s">
         <v>54</v>
@@ -74813,7 +74813,7 @@
         <v>52</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I76" s="13" t="s">
         <v>54</v>
@@ -74855,7 +74855,7 @@
         <v>52</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I77" s="13" t="s">
         <v>54</v>
@@ -74897,7 +74897,7 @@
         <v>52</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>54</v>
@@ -74939,7 +74939,7 @@
         <v>52</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>54</v>
@@ -74981,7 +74981,7 @@
         <v>52</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>54</v>
@@ -75023,7 +75023,7 @@
         <v>52</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>54</v>
@@ -75065,7 +75065,7 @@
         <v>52</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I82" s="13" t="s">
         <v>54</v>
@@ -75107,7 +75107,7 @@
         <v>52</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I83" s="13" t="s">
         <v>54</v>
@@ -75149,7 +75149,7 @@
         <v>52</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I84" s="13" t="s">
         <v>54</v>
@@ -75191,7 +75191,7 @@
         <v>52</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>54</v>
@@ -75233,7 +75233,7 @@
         <v>52</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I86" s="13" t="s">
         <v>54</v>
@@ -75275,7 +75275,7 @@
         <v>52</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>54</v>
@@ -75317,7 +75317,7 @@
         <v>52</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>54</v>
@@ -75359,7 +75359,7 @@
         <v>52</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I89" s="13" t="s">
         <v>54</v>
@@ -75401,7 +75401,7 @@
         <v>52</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>54</v>
@@ -75443,7 +75443,7 @@
         <v>52</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>54</v>
@@ -75485,7 +75485,7 @@
         <v>52</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I92" s="13" t="s">
         <v>54</v>
@@ -75527,7 +75527,7 @@
         <v>52</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I93" s="13" t="s">
         <v>54</v>
@@ -75569,7 +75569,7 @@
         <v>52</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I94" s="13" t="s">
         <v>54</v>
@@ -78676,8 +78676,8 @@
       <c r="G168" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H168" s="16" t="s">
-        <v>53</v>
+      <c r="H168" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I168" s="16" t="s">
         <v>54</v>
@@ -78718,8 +78718,8 @@
       <c r="G169" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H169" s="16" t="s">
-        <v>53</v>
+      <c r="H169" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I169" s="16" t="s">
         <v>54</v>
@@ -78760,8 +78760,8 @@
       <c r="G170" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H170" s="16" t="s">
-        <v>53</v>
+      <c r="H170" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I170" s="16" t="s">
         <v>54</v>
@@ -78802,8 +78802,8 @@
       <c r="G171" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H171" s="16" t="s">
-        <v>53</v>
+      <c r="H171" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I171" s="16" t="s">
         <v>54</v>
@@ -78844,8 +78844,8 @@
       <c r="G172" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H172" s="16" t="s">
-        <v>53</v>
+      <c r="H172" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I172" s="16" t="s">
         <v>54</v>
@@ -78886,8 +78886,8 @@
       <c r="G173" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H173" s="16" t="s">
-        <v>53</v>
+      <c r="H173" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I173" s="16" t="s">
         <v>54</v>
@@ -78928,8 +78928,8 @@
       <c r="G174" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H174" s="16" t="s">
-        <v>53</v>
+      <c r="H174" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I174" s="16" t="s">
         <v>54</v>
@@ -78970,8 +78970,8 @@
       <c r="G175" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H175" s="16" t="s">
-        <v>53</v>
+      <c r="H175" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I175" s="16" t="s">
         <v>54</v>
@@ -79012,8 +79012,8 @@
       <c r="G176" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H176" s="16" t="s">
-        <v>53</v>
+      <c r="H176" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I176" s="16" t="s">
         <v>54</v>
@@ -79054,8 +79054,8 @@
       <c r="G177" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H177" s="16" t="s">
-        <v>53</v>
+      <c r="H177" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I177" s="16" t="s">
         <v>54</v>
@@ -79096,8 +79096,8 @@
       <c r="G178" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H178" s="16" t="s">
-        <v>53</v>
+      <c r="H178" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I178" s="16" t="s">
         <v>54</v>
@@ -79138,8 +79138,8 @@
       <c r="G179" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H179" s="16" t="s">
-        <v>53</v>
+      <c r="H179" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I179" s="16" t="s">
         <v>54</v>
@@ -79180,8 +79180,8 @@
       <c r="G180" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H180" s="16" t="s">
-        <v>53</v>
+      <c r="H180" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I180" s="16" t="s">
         <v>54</v>
@@ -79222,8 +79222,8 @@
       <c r="G181" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H181" s="16" t="s">
-        <v>53</v>
+      <c r="H181" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I181" s="16" t="s">
         <v>54</v>
@@ -79264,8 +79264,8 @@
       <c r="G182" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H182" s="16" t="s">
-        <v>53</v>
+      <c r="H182" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I182" s="16" t="s">
         <v>54</v>
@@ -79307,7 +79307,7 @@
         <v>52</v>
       </c>
       <c r="H183" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I183" t="s">
         <v>54</v>
@@ -79349,7 +79349,7 @@
         <v>52</v>
       </c>
       <c r="H184" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I184" t="s">
         <v>54</v>
@@ -79391,7 +79391,7 @@
         <v>52</v>
       </c>
       <c r="H185" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I185" t="s">
         <v>54</v>
@@ -79433,7 +79433,7 @@
         <v>52</v>
       </c>
       <c r="H186" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="I186" t="s">
         <v>54</v>
@@ -79474,8 +79474,8 @@
       <c r="G187" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H187" s="16" t="s">
-        <v>53</v>
+      <c r="H187" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I187" s="16" t="s">
         <v>54</v>
@@ -79516,8 +79516,8 @@
       <c r="G188" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H188" s="16" t="s">
-        <v>53</v>
+      <c r="H188" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I188" s="16" t="s">
         <v>54</v>
@@ -79558,8 +79558,8 @@
       <c r="G189" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H189" s="16" t="s">
-        <v>53</v>
+      <c r="H189" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I189" s="16" t="s">
         <v>54</v>
@@ -79600,8 +79600,8 @@
       <c r="G190" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H190" s="16" t="s">
-        <v>53</v>
+      <c r="H190" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I190" s="16" t="s">
         <v>54</v>
@@ -79642,8 +79642,8 @@
       <c r="G191" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H191" s="16" t="s">
-        <v>53</v>
+      <c r="H191" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I191" s="16" t="s">
         <v>54</v>
@@ -79684,8 +79684,8 @@
       <c r="G192" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H192" s="16" t="s">
-        <v>53</v>
+      <c r="H192" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I192" s="16" t="s">
         <v>54</v>
@@ -79726,8 +79726,8 @@
       <c r="G193" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H193" s="16" t="s">
-        <v>53</v>
+      <c r="H193" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I193" s="16" t="s">
         <v>54</v>
@@ -79768,8 +79768,8 @@
       <c r="G194" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H194" s="16" t="s">
-        <v>53</v>
+      <c r="H194" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I194" s="16" t="s">
         <v>54</v>
@@ -79810,8 +79810,8 @@
       <c r="G195" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H195" s="16" t="s">
-        <v>53</v>
+      <c r="H195" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I195" s="16" t="s">
         <v>54</v>
@@ -79852,8 +79852,8 @@
       <c r="G196" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H196" s="16" t="s">
-        <v>53</v>
+      <c r="H196" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I196" s="16" t="s">
         <v>54</v>
@@ -79894,8 +79894,8 @@
       <c r="G197" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H197" s="18" t="s">
-        <v>53</v>
+      <c r="H197" t="s">
+        <v>219</v>
       </c>
       <c r="I197" s="18" t="s">
         <v>54</v>
@@ -79936,8 +79936,8 @@
       <c r="G198" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H198" s="18" t="s">
-        <v>53</v>
+      <c r="H198" t="s">
+        <v>219</v>
       </c>
       <c r="I198" s="18" t="s">
         <v>54</v>
@@ -79978,8 +79978,8 @@
       <c r="G199" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H199" s="18" t="s">
-        <v>53</v>
+      <c r="H199" t="s">
+        <v>219</v>
       </c>
       <c r="I199" s="18" t="s">
         <v>54</v>
@@ -80020,8 +80020,8 @@
       <c r="G200" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H200" s="18" t="s">
-        <v>53</v>
+      <c r="H200" t="s">
+        <v>219</v>
       </c>
       <c r="I200" s="18" t="s">
         <v>54</v>
@@ -80062,8 +80062,8 @@
       <c r="G201" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H201" s="18" t="s">
-        <v>53</v>
+      <c r="H201" t="s">
+        <v>219</v>
       </c>
       <c r="I201" s="18" t="s">
         <v>54</v>
@@ -80104,8 +80104,8 @@
       <c r="G202" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H202" s="18" t="s">
-        <v>53</v>
+      <c r="H202" t="s">
+        <v>219</v>
       </c>
       <c r="I202" s="18" t="s">
         <v>54</v>
@@ -80146,8 +80146,8 @@
       <c r="G203" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H203" s="18" t="s">
-        <v>53</v>
+      <c r="H203" t="s">
+        <v>219</v>
       </c>
       <c r="I203" s="18" t="s">
         <v>54</v>
@@ -80188,8 +80188,8 @@
       <c r="G204" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H204" s="18" t="s">
-        <v>53</v>
+      <c r="H204" t="s">
+        <v>219</v>
       </c>
       <c r="I204" s="18" t="s">
         <v>54</v>
@@ -80230,8 +80230,8 @@
       <c r="G205" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H205" s="18" t="s">
-        <v>53</v>
+      <c r="H205" t="s">
+        <v>219</v>
       </c>
       <c r="I205" s="18" t="s">
         <v>54</v>
@@ -80272,8 +80272,8 @@
       <c r="G206" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H206" s="18" t="s">
-        <v>53</v>
+      <c r="H206" t="s">
+        <v>219</v>
       </c>
       <c r="I206" s="18" t="s">
         <v>54</v>
@@ -80314,8 +80314,8 @@
       <c r="G207" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H207" s="16" t="s">
-        <v>53</v>
+      <c r="H207" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I207" s="16" t="s">
         <v>54</v>
@@ -80356,8 +80356,8 @@
       <c r="G208" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H208" s="16" t="s">
-        <v>53</v>
+      <c r="H208" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I208" s="16" t="s">
         <v>54</v>
@@ -80398,8 +80398,8 @@
       <c r="G209" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H209" s="16" t="s">
-        <v>53</v>
+      <c r="H209" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I209" s="16" t="s">
         <v>54</v>
@@ -80440,8 +80440,8 @@
       <c r="G210" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H210" s="16" t="s">
-        <v>53</v>
+      <c r="H210" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I210" s="16" t="s">
         <v>54</v>
@@ -80482,8 +80482,8 @@
       <c r="G211" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H211" s="16" t="s">
-        <v>53</v>
+      <c r="H211" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I211" s="16" t="s">
         <v>54</v>
@@ -80524,8 +80524,8 @@
       <c r="G212" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H212" s="16" t="s">
-        <v>53</v>
+      <c r="H212" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I212" s="16" t="s">
         <v>54</v>
@@ -80566,8 +80566,8 @@
       <c r="G213" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H213" s="16" t="s">
-        <v>53</v>
+      <c r="H213" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I213" s="16" t="s">
         <v>54</v>
@@ -80608,8 +80608,8 @@
       <c r="G214" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H214" s="16" t="s">
-        <v>53</v>
+      <c r="H214" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I214" s="16" t="s">
         <v>54</v>
@@ -80650,8 +80650,8 @@
       <c r="G215" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H215" s="16" t="s">
-        <v>53</v>
+      <c r="H215" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I215" s="16" t="s">
         <v>54</v>
@@ -80692,8 +80692,8 @@
       <c r="G216" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H216" s="16" t="s">
-        <v>53</v>
+      <c r="H216" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I216" s="16" t="s">
         <v>54</v>
@@ -80734,8 +80734,8 @@
       <c r="G217" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H217" s="16" t="s">
-        <v>53</v>
+      <c r="H217" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I217" s="16" t="s">
         <v>54</v>
@@ -80776,8 +80776,8 @@
       <c r="G218" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H218" s="16" t="s">
-        <v>53</v>
+      <c r="H218" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I218" s="16" t="s">
         <v>54</v>
@@ -80818,8 +80818,8 @@
       <c r="G219" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H219" s="16" t="s">
-        <v>53</v>
+      <c r="H219" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I219" s="16" t="s">
         <v>54</v>
@@ -80860,8 +80860,8 @@
       <c r="G220" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H220" s="16" t="s">
-        <v>53</v>
+      <c r="H220" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I220" s="16" t="s">
         <v>54</v>
@@ -80902,8 +80902,8 @@
       <c r="G221" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H221" s="16" t="s">
-        <v>53</v>
+      <c r="H221" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I221" s="16" t="s">
         <v>54</v>
@@ -80944,8 +80944,8 @@
       <c r="G222" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H222" s="16" t="s">
-        <v>53</v>
+      <c r="H222" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I222" s="16" t="s">
         <v>54</v>
@@ -80986,8 +80986,8 @@
       <c r="G223" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H223" s="16" t="s">
-        <v>53</v>
+      <c r="H223" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I223" s="16" t="s">
         <v>54</v>
@@ -81028,8 +81028,8 @@
       <c r="G224" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H224" s="16" t="s">
-        <v>53</v>
+      <c r="H224" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I224" s="16" t="s">
         <v>54</v>
@@ -81070,8 +81070,8 @@
       <c r="G225" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H225" s="16" t="s">
-        <v>53</v>
+      <c r="H225" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I225" s="16" t="s">
         <v>54</v>
@@ -81112,8 +81112,8 @@
       <c r="G226" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H226" s="16" t="s">
-        <v>53</v>
+      <c r="H226" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I226" s="16" t="s">
         <v>54</v>
@@ -81154,8 +81154,8 @@
       <c r="G227" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H227" s="16" t="s">
-        <v>53</v>
+      <c r="H227" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I227" s="16" t="s">
         <v>54</v>
@@ -81196,8 +81196,8 @@
       <c r="G228" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H228" s="18" t="s">
-        <v>53</v>
+      <c r="H228" t="s">
+        <v>219</v>
       </c>
       <c r="I228" s="18" t="s">
         <v>54</v>
@@ -81238,8 +81238,8 @@
       <c r="G229" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H229" s="18" t="s">
-        <v>53</v>
+      <c r="H229" t="s">
+        <v>219</v>
       </c>
       <c r="I229" s="18" t="s">
         <v>54</v>
@@ -81280,8 +81280,8 @@
       <c r="G230" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H230" s="18" t="s">
-        <v>53</v>
+      <c r="H230" t="s">
+        <v>219</v>
       </c>
       <c r="I230" s="18" t="s">
         <v>54</v>
@@ -81322,8 +81322,8 @@
       <c r="G231" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H231" s="16" t="s">
-        <v>53</v>
+      <c r="H231" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I231" s="16" t="s">
         <v>54</v>
@@ -81364,8 +81364,8 @@
       <c r="G232" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H232" s="16" t="s">
-        <v>53</v>
+      <c r="H232" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I232" s="16" t="s">
         <v>54</v>
@@ -81406,8 +81406,8 @@
       <c r="G233" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H233" s="16" t="s">
-        <v>53</v>
+      <c r="H233" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I233" s="16" t="s">
         <v>54</v>
@@ -81448,8 +81448,8 @@
       <c r="G234" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H234" s="16" t="s">
-        <v>53</v>
+      <c r="H234" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I234" s="16" t="s">
         <v>54</v>
@@ -81490,8 +81490,8 @@
       <c r="G235" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H235" s="16" t="s">
-        <v>53</v>
+      <c r="H235" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I235" s="16" t="s">
         <v>54</v>
@@ -81532,8 +81532,8 @@
       <c r="G236" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H236" s="16" t="s">
-        <v>53</v>
+      <c r="H236" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I236" s="16" t="s">
         <v>54</v>
@@ -81574,8 +81574,8 @@
       <c r="G237" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H237" s="16" t="s">
-        <v>53</v>
+      <c r="H237" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I237" s="16" t="s">
         <v>54</v>
@@ -81616,8 +81616,8 @@
       <c r="G238" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H238" s="16" t="s">
-        <v>53</v>
+      <c r="H238" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I238" s="16" t="s">
         <v>54</v>
@@ -81658,8 +81658,8 @@
       <c r="G239" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H239" s="16" t="s">
-        <v>53</v>
+      <c r="H239" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I239" s="16" t="s">
         <v>54</v>
@@ -81700,8 +81700,8 @@
       <c r="G240" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H240" s="16" t="s">
-        <v>53</v>
+      <c r="H240" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I240" s="16" t="s">
         <v>54</v>
@@ -81742,8 +81742,8 @@
       <c r="G241" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H241" s="16" t="s">
-        <v>53</v>
+      <c r="H241" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I241" s="16" t="s">
         <v>54</v>
@@ -81784,8 +81784,8 @@
       <c r="G242" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H242" s="16" t="s">
-        <v>53</v>
+      <c r="H242" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I242" s="16" t="s">
         <v>54</v>
@@ -81826,8 +81826,8 @@
       <c r="G243" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H243" s="16" t="s">
-        <v>53</v>
+      <c r="H243" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I243" s="16" t="s">
         <v>54</v>
@@ -81868,8 +81868,8 @@
       <c r="G244" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H244" s="16" t="s">
-        <v>53</v>
+      <c r="H244" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I244" s="16" t="s">
         <v>54</v>
@@ -81910,8 +81910,8 @@
       <c r="G245" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H245" s="16" t="s">
-        <v>53</v>
+      <c r="H245" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I245" s="16" t="s">
         <v>54</v>
@@ -81952,8 +81952,8 @@
       <c r="G246" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H246" s="16" t="s">
-        <v>53</v>
+      <c r="H246" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I246" s="16" t="s">
         <v>54</v>
@@ -81994,8 +81994,8 @@
       <c r="G247" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H247" s="16" t="s">
-        <v>53</v>
+      <c r="H247" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I247" s="16" t="s">
         <v>54</v>
@@ -82036,8 +82036,8 @@
       <c r="G248" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H248" s="16" t="s">
-        <v>53</v>
+      <c r="H248" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I248" s="16" t="s">
         <v>54</v>
@@ -82078,8 +82078,8 @@
       <c r="G249" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H249" s="16" t="s">
-        <v>53</v>
+      <c r="H249" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I249" s="16" t="s">
         <v>54</v>
@@ -82120,8 +82120,8 @@
       <c r="G250" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H250" s="16" t="s">
-        <v>53</v>
+      <c r="H250" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I250" s="16" t="s">
         <v>54</v>
@@ -82162,8 +82162,8 @@
       <c r="G251" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H251" s="16" t="s">
-        <v>53</v>
+      <c r="H251" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I251" s="16" t="s">
         <v>54</v>
@@ -82204,8 +82204,8 @@
       <c r="G252" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H252" s="16" t="s">
-        <v>53</v>
+      <c r="H252" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I252" s="16" t="s">
         <v>54</v>
@@ -82246,8 +82246,8 @@
       <c r="G253" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H253" s="16" t="s">
-        <v>53</v>
+      <c r="H253" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I253" s="16" t="s">
         <v>54</v>
@@ -82288,8 +82288,8 @@
       <c r="G254" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H254" s="16" t="s">
-        <v>53</v>
+      <c r="H254" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I254" s="16" t="s">
         <v>54</v>
@@ -82330,8 +82330,8 @@
       <c r="G255" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H255" s="16" t="s">
-        <v>53</v>
+      <c r="H255" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I255" s="16" t="s">
         <v>54</v>
@@ -82372,8 +82372,8 @@
       <c r="G256" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H256" s="16" t="s">
-        <v>53</v>
+      <c r="H256" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I256" s="16" t="s">
         <v>54</v>
@@ -82414,8 +82414,8 @@
       <c r="G257" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H257" s="16" t="s">
-        <v>53</v>
+      <c r="H257" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I257" s="16" t="s">
         <v>54</v>
@@ -82456,8 +82456,8 @@
       <c r="G258" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H258" s="16" t="s">
-        <v>53</v>
+      <c r="H258" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I258" s="16" t="s">
         <v>54</v>
@@ -82498,8 +82498,8 @@
       <c r="G259" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H259" s="16" t="s">
-        <v>53</v>
+      <c r="H259" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I259" s="16" t="s">
         <v>54</v>
@@ -82540,8 +82540,8 @@
       <c r="G260" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H260" s="16" t="s">
-        <v>53</v>
+      <c r="H260" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I260" s="16" t="s">
         <v>54</v>
@@ -82582,8 +82582,8 @@
       <c r="G261" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H261" s="16" t="s">
-        <v>53</v>
+      <c r="H261" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I261" s="16" t="s">
         <v>54</v>
@@ -82624,8 +82624,8 @@
       <c r="G262" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H262" s="16" t="s">
-        <v>53</v>
+      <c r="H262" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I262" s="16" t="s">
         <v>54</v>
@@ -82666,8 +82666,8 @@
       <c r="G263" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H263" s="16" t="s">
-        <v>53</v>
+      <c r="H263" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I263" s="16" t="s">
         <v>54</v>
@@ -82708,8 +82708,8 @@
       <c r="G264" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H264" s="16" t="s">
-        <v>53</v>
+      <c r="H264" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I264" s="16" t="s">
         <v>54</v>
@@ -82750,8 +82750,8 @@
       <c r="G265" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H265" s="16" t="s">
-        <v>53</v>
+      <c r="H265" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I265" s="16" t="s">
         <v>54</v>
@@ -82792,8 +82792,8 @@
       <c r="G266" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H266" s="16" t="s">
-        <v>53</v>
+      <c r="H266" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I266" s="16" t="s">
         <v>54</v>
@@ -82834,8 +82834,8 @@
       <c r="G267" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H267" s="16" t="s">
-        <v>53</v>
+      <c r="H267" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I267" s="16" t="s">
         <v>54</v>
@@ -82876,8 +82876,8 @@
       <c r="G268" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H268" s="16" t="s">
-        <v>53</v>
+      <c r="H268" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I268" s="16" t="s">
         <v>54</v>
@@ -82918,8 +82918,8 @@
       <c r="G269" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H269" s="16" t="s">
-        <v>53</v>
+      <c r="H269" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I269" s="16" t="s">
         <v>54</v>
@@ -82960,8 +82960,8 @@
       <c r="G270" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H270" s="16" t="s">
-        <v>53</v>
+      <c r="H270" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I270" s="16" t="s">
         <v>54</v>
@@ -83002,8 +83002,8 @@
       <c r="G271" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H271" s="16" t="s">
-        <v>53</v>
+      <c r="H271" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I271" s="16" t="s">
         <v>54</v>
@@ -83044,8 +83044,8 @@
       <c r="G272" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H272" s="16" t="s">
-        <v>53</v>
+      <c r="H272" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I272" s="16" t="s">
         <v>54</v>
@@ -83086,8 +83086,8 @@
       <c r="G273" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H273" s="16" t="s">
-        <v>53</v>
+      <c r="H273" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I273" s="16" t="s">
         <v>54</v>
@@ -83128,8 +83128,8 @@
       <c r="G274" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H274" s="16" t="s">
-        <v>53</v>
+      <c r="H274" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I274" s="16" t="s">
         <v>54</v>
@@ -83170,8 +83170,8 @@
       <c r="G275" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H275" s="16" t="s">
-        <v>53</v>
+      <c r="H275" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I275" s="16" t="s">
         <v>54</v>
@@ -83212,8 +83212,8 @@
       <c r="G276" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H276" s="16" t="s">
-        <v>53</v>
+      <c r="H276" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I276" s="16" t="s">
         <v>54</v>
@@ -83254,8 +83254,8 @@
       <c r="G277" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H277" s="16" t="s">
-        <v>53</v>
+      <c r="H277" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I277" s="16" t="s">
         <v>54</v>
@@ -83296,8 +83296,8 @@
       <c r="G278" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H278" s="16" t="s">
-        <v>53</v>
+      <c r="H278" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I278" s="16" t="s">
         <v>54</v>
@@ -83338,8 +83338,8 @@
       <c r="G279" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H279" s="16" t="s">
-        <v>53</v>
+      <c r="H279" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I279" s="16" t="s">
         <v>54</v>
@@ -83380,8 +83380,8 @@
       <c r="G280" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H280" s="16" t="s">
-        <v>53</v>
+      <c r="H280" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I280" s="16" t="s">
         <v>54</v>

</xml_diff>